<commit_message>
combine IV bydischarge and byhicbic do files into loops
</commit_message>
<xml_diff>
--- a/do/MA_reg.xlsx
+++ b/do/MA_reg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="14920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="bene-level" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8204" uniqueCount="2460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8204" uniqueCount="2471">
   <si>
     <t/>
   </si>
@@ -7400,7 +7400,40 @@
     <t>ma_hat_teach</t>
   </si>
   <si>
-    <t>teaching</t>
+    <t>ma_CAP_pat_k_star</t>
+  </si>
+  <si>
+    <t>ma_np_pat_k_star</t>
+  </si>
+  <si>
+    <t>ma_fp_pat_k_star</t>
+  </si>
+  <si>
+    <t>ma_small_pat_k_star</t>
+  </si>
+  <si>
+    <t>ma_med_pat_k_star</t>
+  </si>
+  <si>
+    <t>ma_teach_pat_k_star</t>
+  </si>
+  <si>
+    <t>CAP_pat_k_star</t>
+  </si>
+  <si>
+    <t>fp_pat_k_star</t>
+  </si>
+  <si>
+    <t>np_pat_k_star</t>
+  </si>
+  <si>
+    <t>small_pat_k_star</t>
+  </si>
+  <si>
+    <t>med_pat_k_star</t>
+  </si>
+  <si>
+    <t>teaching_pat_k_star</t>
   </si>
 </sst>
 </file>
@@ -7662,13 +7695,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="204">
+  <cellStyleXfs count="248">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7944,7 +8021,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="204">
+  <cellStyles count="248">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -8046,6 +8123,28 @@
     <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -8147,6 +8246,28 @@
     <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5"/>
   </cellStyles>
@@ -8479,8 +8600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K230" sqref="K230"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9077,7 +9198,7 @@
     </row>
     <row r="20" spans="1:21" s="12" customFormat="1">
       <c r="A20" s="14" t="s">
-        <v>2443</v>
+        <v>2459</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>0</v>
@@ -9207,7 +9328,7 @@
     </row>
     <row r="22" spans="1:21" s="12" customFormat="1">
       <c r="A22" s="14" t="s">
-        <v>2445</v>
+        <v>2460</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>0</v>
@@ -9337,7 +9458,7 @@
     </row>
     <row r="24" spans="1:21" s="12" customFormat="1">
       <c r="A24" s="14" t="s">
-        <v>2444</v>
+        <v>2461</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>0</v>
@@ -9467,7 +9588,7 @@
     </row>
     <row r="26" spans="1:21" s="12" customFormat="1">
       <c r="A26" s="14" t="s">
-        <v>2447</v>
+        <v>2462</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>0</v>
@@ -9597,7 +9718,7 @@
     </row>
     <row r="28" spans="1:21" s="12" customFormat="1">
       <c r="A28" s="14" t="s">
-        <v>2448</v>
+        <v>2463</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>0</v>
@@ -9727,7 +9848,7 @@
     </row>
     <row r="30" spans="1:21" s="12" customFormat="1">
       <c r="A30" s="14" t="s">
-        <v>2450</v>
+        <v>2464</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>0</v>
@@ -9987,7 +10108,7 @@
     </row>
     <row r="34" spans="1:21" s="12" customFormat="1">
       <c r="A34" s="14" t="s">
-        <v>2435</v>
+        <v>2465</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>1260</v>
@@ -10117,7 +10238,7 @@
     </row>
     <row r="36" spans="1:21" s="12" customFormat="1">
       <c r="A36" s="14" t="s">
-        <v>2436</v>
+        <v>2466</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>1296</v>
@@ -10247,7 +10368,7 @@
     </row>
     <row r="38" spans="1:21" s="12" customFormat="1">
       <c r="A38" s="14" t="s">
-        <v>2437</v>
+        <v>2467</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>1315</v>
@@ -10377,7 +10498,7 @@
     </row>
     <row r="40" spans="1:21" s="12" customFormat="1">
       <c r="A40" s="14" t="s">
-        <v>2439</v>
+        <v>2468</v>
       </c>
       <c r="B40" s="14" t="s">
         <v>1331</v>
@@ -10507,7 +10628,7 @@
     </row>
     <row r="42" spans="1:21" s="12" customFormat="1">
       <c r="A42" s="14" t="s">
-        <v>2440</v>
+        <v>2469</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>1350</v>
@@ -10637,7 +10758,7 @@
     </row>
     <row r="44" spans="1:21" s="12" customFormat="1">
       <c r="A44" s="14" t="s">
-        <v>2459</v>
+        <v>2470</v>
       </c>
       <c r="B44" s="14" t="s">
         <v>1367</v>
@@ -22721,6 +22842,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -22733,8 +22855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P229"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C222" sqref="C222"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -23250,7 +23372,7 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="14" t="s">
-        <v>2443</v>
+        <v>2459</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>0</v>
@@ -23350,7 +23472,7 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="14" t="s">
-        <v>2444</v>
+        <v>2460</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>0</v>
@@ -23450,7 +23572,7 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="14" t="s">
-        <v>2445</v>
+        <v>2461</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>0</v>
@@ -23550,7 +23672,7 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="14" t="s">
-        <v>2447</v>
+        <v>2462</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>0</v>
@@ -23650,7 +23772,7 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="14" t="s">
-        <v>2448</v>
+        <v>2463</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>0</v>
@@ -23750,7 +23872,7 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="14" t="s">
-        <v>2450</v>
+        <v>2464</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>0</v>
@@ -23950,7 +24072,7 @@
     </row>
     <row r="34" spans="1:16">
       <c r="A34" s="14" t="s">
-        <v>2435</v>
+        <v>2465</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>1617</v>
@@ -24050,7 +24172,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="14" t="s">
-        <v>2436</v>
+        <v>2466</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>1640</v>
@@ -24150,7 +24272,7 @@
     </row>
     <row r="38" spans="1:16">
       <c r="A38" s="14" t="s">
-        <v>2437</v>
+        <v>2467</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>964</v>
@@ -24250,7 +24372,7 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="14" t="s">
-        <v>2439</v>
+        <v>2468</v>
       </c>
       <c r="B40" s="14" t="s">
         <v>1661</v>
@@ -24350,7 +24472,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="14" t="s">
-        <v>2440</v>
+        <v>2469</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>150</v>
@@ -24450,7 +24572,7 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="14" t="s">
-        <v>2442</v>
+        <v>2470</v>
       </c>
       <c r="B44" s="14" t="s">
         <v>478</v>
@@ -33756,8 +33878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="J121" sqref="J121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -33870,16 +33992,16 @@
       <c r="I3" s="28">
         <v>1</v>
       </c>
-      <c r="J3" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="K3" s="10">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="L3" s="10">
-        <v>0</v>
-      </c>
-      <c r="M3" s="17">
+      <c r="J3">
+        <v>0.1504798</v>
+      </c>
+      <c r="K3">
+        <v>0.3575411</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
         <v>1</v>
       </c>
     </row>
@@ -33911,16 +34033,16 @@
       <c r="I4" s="31">
         <v>1</v>
       </c>
-      <c r="J4" s="12">
-        <v>0.28299999999999997</v>
-      </c>
-      <c r="K4" s="12">
-        <v>0.13</v>
-      </c>
-      <c r="L4" s="12">
-        <v>0</v>
-      </c>
-      <c r="M4" s="18">
+      <c r="J4">
+        <v>0.28255200000000003</v>
+      </c>
+      <c r="K4">
+        <v>0.13012280000000001</v>
+      </c>
+      <c r="L4">
+        <v>8.6478899999999997E-2</v>
+      </c>
+      <c r="M4">
         <v>1</v>
       </c>
     </row>
@@ -33952,17 +34074,17 @@
       <c r="I5" s="31">
         <v>352442.5</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5">
         <v>63424.09</v>
       </c>
-      <c r="K5" s="12">
-        <v>47308.983999999997</v>
-      </c>
-      <c r="L5" s="12">
-        <v>321</v>
-      </c>
-      <c r="M5" s="18">
-        <v>352443</v>
+      <c r="K5">
+        <v>47308.98</v>
+      </c>
+      <c r="L5">
+        <v>321.09140000000002</v>
+      </c>
+      <c r="M5">
+        <v>352442.5</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -33993,17 +34115,17 @@
       <c r="I6" s="31">
         <v>0.98261960000000004</v>
       </c>
-      <c r="J6" s="12">
-        <v>0.155</v>
-      </c>
-      <c r="K6" s="12">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="L6" s="12">
-        <v>0</v>
-      </c>
-      <c r="M6" s="18">
-        <v>1</v>
+      <c r="J6">
+        <v>0.15450810000000001</v>
+      </c>
+      <c r="K6">
+        <v>0.17654529999999999</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0.98261960000000004</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -34034,16 +34156,16 @@
       <c r="I7" s="31">
         <v>1</v>
       </c>
-      <c r="J7" s="12">
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="K7" s="12">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="L7" s="12">
-        <v>0</v>
-      </c>
-      <c r="M7" s="18">
+      <c r="J7">
+        <v>0.75703940000000003</v>
+      </c>
+      <c r="K7">
+        <v>0.22851299999999999</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
         <v>1</v>
       </c>
     </row>
@@ -34075,16 +34197,16 @@
       <c r="I8" s="31">
         <v>1</v>
       </c>
-      <c r="J8" s="12">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="K8" s="12">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="L8" s="12">
-        <v>0</v>
-      </c>
-      <c r="M8" s="18">
+      <c r="J8">
+        <v>8.8452500000000003E-2</v>
+      </c>
+      <c r="K8">
+        <v>0.13133210000000001</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
         <v>1</v>
       </c>
     </row>
@@ -34116,16 +34238,16 @@
       <c r="I9" s="31">
         <v>1</v>
       </c>
-      <c r="J9" s="12">
-        <v>0.128</v>
-      </c>
-      <c r="K9" s="12">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="L9" s="12">
-        <v>0</v>
-      </c>
-      <c r="M9" s="18">
+      <c r="J9">
+        <v>0.12844159999999999</v>
+      </c>
+      <c r="K9">
+        <v>0.13256039999999999</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
         <v>1</v>
       </c>
     </row>
@@ -34157,16 +34279,16 @@
       <c r="I10" s="31">
         <v>1</v>
       </c>
-      <c r="J10" s="12">
-        <v>0.69399999999999995</v>
-      </c>
-      <c r="K10" s="12">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="L10" s="12">
-        <v>0</v>
-      </c>
-      <c r="M10" s="18">
+      <c r="J10">
+        <v>0.69412229999999997</v>
+      </c>
+      <c r="K10">
+        <v>0.1761171</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
         <v>1</v>
       </c>
     </row>
@@ -34198,17 +34320,17 @@
       <c r="I11" s="31">
         <v>0.83372590000000002</v>
       </c>
-      <c r="J11" s="12">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="K11" s="12">
-        <v>0.16</v>
-      </c>
-      <c r="L11" s="12">
-        <v>0</v>
-      </c>
-      <c r="M11" s="18">
-        <v>1</v>
+      <c r="J11">
+        <v>0.17743610000000001</v>
+      </c>
+      <c r="K11">
+        <v>0.16019990000000001</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0.83372590000000002</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -34239,17 +34361,17 @@
       <c r="I12" s="31">
         <v>0.99873979999999996</v>
       </c>
-      <c r="J12" s="12">
-        <v>0.51900000000000002</v>
-      </c>
-      <c r="K12" s="12">
-        <v>0.248</v>
-      </c>
-      <c r="L12" s="12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="18">
-        <v>1</v>
+      <c r="J12">
+        <v>0.5190091</v>
+      </c>
+      <c r="K12">
+        <v>0.24847330000000001</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0.99873979999999996</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -34280,16 +34402,16 @@
       <c r="I13" s="31">
         <v>1</v>
       </c>
-      <c r="J13" s="12">
-        <v>0.04</v>
-      </c>
-      <c r="K13" s="12">
-        <v>0.105</v>
-      </c>
-      <c r="L13" s="12">
-        <v>0</v>
-      </c>
-      <c r="M13" s="18">
+      <c r="J13">
+        <v>4.0048500000000001E-2</v>
+      </c>
+      <c r="K13">
+        <v>0.1048164</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
         <v>1</v>
       </c>
     </row>
@@ -34321,17 +34443,17 @@
       <c r="I14" s="31">
         <v>352442.5</v>
       </c>
-      <c r="J14" s="12">
-        <v>10122.314</v>
-      </c>
-      <c r="K14" s="12">
-        <v>30411.532999999999</v>
-      </c>
-      <c r="L14" s="12">
-        <v>0</v>
-      </c>
-      <c r="M14" s="18">
-        <v>352443</v>
+      <c r="J14">
+        <v>10122.31</v>
+      </c>
+      <c r="K14">
+        <v>30411.53</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>352442.5</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -34362,17 +34484,17 @@
       <c r="I15" s="31">
         <v>0.98261960000000004</v>
       </c>
-      <c r="J15" s="12">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="K15" s="12">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="L15" s="12">
-        <v>0</v>
-      </c>
-      <c r="M15" s="18">
-        <v>1</v>
+      <c r="J15">
+        <v>2.1067800000000001E-2</v>
+      </c>
+      <c r="K15">
+        <v>8.4652900000000003E-2</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0.98261960000000004</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -34403,16 +34525,16 @@
       <c r="I16" s="31">
         <v>1</v>
       </c>
-      <c r="J16" s="12">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="K16" s="12">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="L16" s="12">
-        <v>0</v>
-      </c>
-      <c r="M16" s="18">
+      <c r="J16">
+        <v>0.1189544</v>
+      </c>
+      <c r="K16">
+        <v>0.2936724</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
         <v>1</v>
       </c>
     </row>
@@ -34444,16 +34566,16 @@
       <c r="I17" s="31">
         <v>1</v>
       </c>
-      <c r="J17" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="K17" s="12">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="L17" s="12">
-        <v>0</v>
-      </c>
-      <c r="M17" s="18">
+      <c r="J17">
+        <v>1.04575E-2</v>
+      </c>
+      <c r="K17">
+        <v>4.4617700000000003E-2</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
         <v>1</v>
       </c>
     </row>
@@ -34485,16 +34607,16 @@
       <c r="I18" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="12">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="K18" s="12">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="L18" s="12">
-        <v>0</v>
-      </c>
-      <c r="M18" s="18">
+      <c r="J18">
+        <v>1.4782E-2</v>
+      </c>
+      <c r="K18">
+        <v>5.17438E-2</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
         <v>1</v>
       </c>
     </row>
@@ -34526,16 +34648,16 @@
       <c r="I19" s="31">
         <v>1</v>
       </c>
-      <c r="J19" s="12">
-        <v>0.105</v>
-      </c>
-      <c r="K19" s="12">
-        <v>0.25600000000000001</v>
-      </c>
-      <c r="L19" s="12">
-        <v>0</v>
-      </c>
-      <c r="M19" s="18">
+      <c r="J19">
+        <v>0.1045078</v>
+      </c>
+      <c r="K19">
+        <v>0.256216</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
         <v>1</v>
       </c>
     </row>
@@ -34567,17 +34689,17 @@
       <c r="I20" s="31">
         <v>0.83372590000000002</v>
       </c>
-      <c r="J20" s="12">
-        <v>3.1E-2</v>
-      </c>
-      <c r="K20" s="12">
-        <v>9.7000000000000003E-2</v>
-      </c>
-      <c r="L20" s="12">
-        <v>0</v>
-      </c>
-      <c r="M20" s="18">
-        <v>1</v>
+      <c r="J20">
+        <v>3.1189999999999999E-2</v>
+      </c>
+      <c r="K20">
+        <v>9.7040000000000001E-2</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0.83372590000000002</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -34608,17 +34730,17 @@
       <c r="I21" s="31">
         <v>0.99873979999999996</v>
       </c>
-      <c r="J21" s="12">
-        <v>8.8999999999999996E-2</v>
-      </c>
-      <c r="K21" s="12">
-        <v>0.23</v>
-      </c>
-      <c r="L21" s="12">
-        <v>0</v>
-      </c>
-      <c r="M21" s="18">
-        <v>1</v>
+      <c r="J21">
+        <v>8.9165700000000001E-2</v>
+      </c>
+      <c r="K21">
+        <v>0.22994590000000001</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0.99873979999999996</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -34649,17 +34771,17 @@
       <c r="I22" s="31">
         <v>0.57665659999999996</v>
       </c>
-      <c r="J22" s="12">
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="K22" s="12">
-        <v>6.2E-2</v>
-      </c>
-      <c r="L22" s="12">
-        <v>0</v>
-      </c>
-      <c r="M22" s="18">
-        <v>0</v>
+      <c r="J22">
+        <v>0.14860090000000001</v>
+      </c>
+      <c r="K22">
+        <v>6.1789200000000002E-2</v>
+      </c>
+      <c r="L22">
+        <v>2.3728999999999998E-3</v>
+      </c>
+      <c r="M22">
+        <v>0.4699989</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -34690,17 +34812,17 @@
       <c r="I23" s="31">
         <v>0.44285380000000002</v>
       </c>
-      <c r="J23" s="12">
-        <v>0.04</v>
-      </c>
-      <c r="K23" s="12">
-        <v>2.3E-2</v>
-      </c>
-      <c r="L23" s="12">
-        <v>0</v>
-      </c>
-      <c r="M23" s="18">
-        <v>0</v>
+      <c r="J23">
+        <v>3.9542599999999997E-2</v>
+      </c>
+      <c r="K23">
+        <v>2.27201E-2</v>
+      </c>
+      <c r="L23">
+        <v>1.1115999999999999E-3</v>
+      </c>
+      <c r="M23">
+        <v>0.32767370000000001</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -34731,17 +34853,17 @@
       <c r="I24" s="31">
         <v>98155.67</v>
       </c>
-      <c r="J24" s="12">
+      <c r="J24">
         <v>9977.7360000000008</v>
       </c>
-      <c r="K24" s="12">
+      <c r="K24">
         <v>9403.6929999999993</v>
       </c>
-      <c r="L24" s="12">
-        <v>6</v>
-      </c>
-      <c r="M24" s="18">
-        <v>92729</v>
+      <c r="L24">
+        <v>6.3692399999999996</v>
+      </c>
+      <c r="M24">
+        <v>92728.93</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -34772,17 +34894,17 @@
       <c r="I25" s="31">
         <v>0.35066560000000002</v>
       </c>
-      <c r="J25" s="12">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="K25" s="12">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="L25" s="12">
-        <v>0</v>
-      </c>
-      <c r="M25" s="18">
-        <v>0</v>
+      <c r="J25">
+        <v>2.06111E-2</v>
+      </c>
+      <c r="K25">
+        <v>2.5559599999999998E-2</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0.2331955</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -34813,17 +34935,17 @@
       <c r="I26" s="31">
         <v>0.458818</v>
       </c>
-      <c r="J26" s="12">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="K26" s="12">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="L26" s="12">
-        <v>0</v>
-      </c>
-      <c r="M26" s="18">
-        <v>0</v>
+      <c r="J26">
+        <v>0.1177598</v>
+      </c>
+      <c r="K26">
+        <v>6.5015799999999999E-2</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0.38281199999999999</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -34854,17 +34976,17 @@
       <c r="I27" s="31">
         <v>0.20394370000000001</v>
       </c>
-      <c r="J27" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="K27" s="12">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="L27" s="12">
-        <v>0</v>
-      </c>
-      <c r="M27" s="18">
-        <v>0</v>
+      <c r="J27">
+        <v>1.023E-2</v>
+      </c>
+      <c r="K27">
+        <v>1.2648899999999999E-2</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0.1889324</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -34895,17 +35017,17 @@
       <c r="I28" s="31">
         <v>0.19722509999999999</v>
       </c>
-      <c r="J28" s="12">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="K28" s="12">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="L28" s="12">
-        <v>0</v>
-      </c>
-      <c r="M28" s="18">
-        <v>0</v>
+      <c r="J28">
+        <v>1.4578300000000001E-2</v>
+      </c>
+      <c r="K28">
+        <v>1.0961200000000001E-2</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0.1286091</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -34936,17 +35058,17 @@
       <c r="I29" s="31">
         <v>0.44285380000000002</v>
       </c>
-      <c r="J29" s="12">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="K29" s="12">
-        <v>4.7E-2</v>
-      </c>
-      <c r="L29" s="12">
-        <v>0</v>
-      </c>
-      <c r="M29" s="18">
-        <v>0</v>
+      <c r="J29">
+        <v>0.1032704</v>
+      </c>
+      <c r="K29">
+        <v>4.71829E-2</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0.34769250000000002</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -34977,17 +35099,17 @@
       <c r="I30" s="31">
         <v>0.27163900000000002</v>
       </c>
-      <c r="J30" s="12">
-        <v>3.1E-2</v>
-      </c>
-      <c r="K30" s="12">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="L30" s="12">
-        <v>0</v>
-      </c>
-      <c r="M30" s="18">
-        <v>0</v>
+      <c r="J30">
+        <v>3.07522E-2</v>
+      </c>
+      <c r="K30">
+        <v>3.4739800000000001E-2</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0.27472570000000002</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -35018,17 +35140,17 @@
       <c r="I31" s="31">
         <v>0.49272670000000002</v>
       </c>
-      <c r="J31" s="12">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="K31" s="12">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="L31" s="12">
-        <v>0</v>
-      </c>
-      <c r="M31" s="18">
-        <v>0</v>
+      <c r="J31">
+        <v>8.8222800000000004E-2</v>
+      </c>
+      <c r="K31">
+        <v>6.8254999999999996E-2</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0.41493229999999998</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -35057,17 +35179,17 @@
       <c r="I32" s="31">
         <v>15.941129999999999</v>
       </c>
-      <c r="J32" s="12">
-        <v>10.026</v>
-      </c>
-      <c r="K32" s="12">
-        <v>0.90900000000000003</v>
-      </c>
-      <c r="L32" s="12">
-        <v>4</v>
-      </c>
-      <c r="M32" s="18">
-        <v>15</v>
+      <c r="J32">
+        <v>10.025829999999999</v>
+      </c>
+      <c r="K32">
+        <v>0.90946930000000004</v>
+      </c>
+      <c r="L32">
+        <v>3.9702920000000002</v>
+      </c>
+      <c r="M32">
+        <v>15.320679999999999</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -35096,17 +35218,17 @@
       <c r="I33" s="31">
         <v>15.07469</v>
       </c>
-      <c r="J33" s="12">
-        <v>8.9570000000000007</v>
-      </c>
-      <c r="K33" s="12">
-        <v>0.84</v>
-      </c>
-      <c r="L33" s="12">
-        <v>4</v>
-      </c>
-      <c r="M33" s="18">
-        <v>15</v>
+      <c r="J33">
+        <v>8.9567530000000009</v>
+      </c>
+      <c r="K33">
+        <v>0.84013769999999999</v>
+      </c>
+      <c r="L33">
+        <v>3.6656569999999999</v>
+      </c>
+      <c r="M33">
+        <v>14.52543</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -35135,17 +35257,17 @@
       <c r="I34" s="31">
         <v>15.927210000000001</v>
       </c>
-      <c r="J34" s="12">
-        <v>8.9789999999999992</v>
-      </c>
-      <c r="K34" s="12">
-        <v>0.66</v>
-      </c>
-      <c r="L34" s="12">
-        <v>1</v>
-      </c>
-      <c r="M34" s="18">
-        <v>16</v>
+      <c r="J34">
+        <v>8.9791170000000005</v>
+      </c>
+      <c r="K34">
+        <v>0.65991639999999996</v>
+      </c>
+      <c r="L34">
+        <v>1.0986119999999999</v>
+      </c>
+      <c r="M34">
+        <v>16.042359999999999</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -35176,16 +35298,16 @@
       <c r="I35" s="31">
         <v>8378118</v>
       </c>
-      <c r="J35" s="12">
-        <v>35368.464</v>
-      </c>
-      <c r="K35" s="12">
-        <v>48696.125999999997</v>
-      </c>
-      <c r="L35" s="12">
+      <c r="J35">
+        <v>35368.46</v>
+      </c>
+      <c r="K35">
+        <v>48696.13</v>
+      </c>
+      <c r="L35">
         <v>53</v>
       </c>
-      <c r="M35" s="18">
+      <c r="M35">
         <v>4504928</v>
       </c>
     </row>
@@ -35217,16 +35339,16 @@
       <c r="I36" s="31">
         <v>3522518</v>
       </c>
-      <c r="J36" s="12">
-        <v>11474.847</v>
-      </c>
-      <c r="K36" s="12">
-        <v>14873.224</v>
-      </c>
-      <c r="L36" s="12">
-        <v>39</v>
-      </c>
-      <c r="M36" s="18">
+      <c r="J36">
+        <v>11474.85</v>
+      </c>
+      <c r="K36">
+        <v>14873.22</v>
+      </c>
+      <c r="L36">
+        <v>39.081780000000002</v>
+      </c>
+      <c r="M36">
         <v>2033828</v>
       </c>
     </row>
@@ -35258,16 +35380,16 @@
       <c r="I37" s="31">
         <v>8262246</v>
       </c>
-      <c r="J37" s="12">
-        <v>10403.177</v>
-      </c>
-      <c r="K37" s="12">
-        <v>15087.727999999999</v>
-      </c>
-      <c r="L37" s="12">
+      <c r="J37">
+        <v>10403.18</v>
+      </c>
+      <c r="K37">
+        <v>15087.73</v>
+      </c>
+      <c r="L37">
         <v>3</v>
       </c>
-      <c r="M37" s="18">
+      <c r="M37">
         <v>9270615</v>
       </c>
     </row>
@@ -35420,16 +35542,16 @@
       <c r="I41" s="31">
         <v>1</v>
       </c>
-      <c r="J41" s="12">
-        <v>0.185</v>
-      </c>
-      <c r="K41" s="12">
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="L41" s="12">
-        <v>0</v>
-      </c>
-      <c r="M41" s="18">
+      <c r="J41">
+        <v>0.1851863</v>
+      </c>
+      <c r="K41">
+        <v>0.38844869999999998</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
         <v>1</v>
       </c>
     </row>
@@ -35461,16 +35583,16 @@
       <c r="I42" s="31">
         <v>1</v>
       </c>
-      <c r="J42" s="12">
-        <v>0.191</v>
-      </c>
-      <c r="K42" s="12">
-        <v>0.39300000000000002</v>
-      </c>
-      <c r="L42" s="12">
-        <v>0</v>
-      </c>
-      <c r="M42" s="18">
+      <c r="J42">
+        <v>0.19132399999999999</v>
+      </c>
+      <c r="K42">
+        <v>0.39334360000000002</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
         <v>1</v>
       </c>
     </row>
@@ -35502,16 +35624,16 @@
       <c r="I43" s="31">
         <v>1</v>
       </c>
-      <c r="J43" s="12">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="K43" s="12">
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="L43" s="12">
-        <v>0</v>
-      </c>
-      <c r="M43" s="18">
+      <c r="J43">
+        <v>0.20661009999999999</v>
+      </c>
+      <c r="K43">
+        <v>0.40487329999999999</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
         <v>1</v>
       </c>
     </row>
@@ -35543,16 +35665,16 @@
       <c r="I44" s="31">
         <v>1</v>
       </c>
-      <c r="J44" s="12">
-        <v>0.34</v>
-      </c>
-      <c r="K44" s="12">
-        <v>0.47399999999999998</v>
-      </c>
-      <c r="L44" s="12">
-        <v>0</v>
-      </c>
-      <c r="M44" s="18">
+      <c r="J44">
+        <v>0.33982400000000001</v>
+      </c>
+      <c r="K44">
+        <v>0.4736493</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
         <v>1</v>
       </c>
     </row>
@@ -35584,16 +35706,16 @@
       <c r="I45" s="31">
         <v>1</v>
       </c>
-      <c r="J45" s="12">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="K45" s="12">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="L45" s="12">
-        <v>0</v>
-      </c>
-      <c r="M45" s="18">
+      <c r="J45">
+        <v>7.7055499999999999E-2</v>
+      </c>
+      <c r="K45">
+        <v>0.26667950000000001</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
         <v>1</v>
       </c>
     </row>
@@ -35625,16 +35747,16 @@
       <c r="I46" s="31">
         <v>1</v>
       </c>
-      <c r="J46" s="12">
-        <v>0.57199999999999995</v>
-      </c>
-      <c r="K46" s="12">
-        <v>0.495</v>
-      </c>
-      <c r="L46" s="12">
-        <v>0</v>
-      </c>
-      <c r="M46" s="18">
+      <c r="J46">
+        <v>0.572241</v>
+      </c>
+      <c r="K46">
+        <v>0.49475370000000002</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
         <v>1</v>
       </c>
     </row>
@@ -35666,16 +35788,16 @@
       <c r="I47" s="31">
         <v>1</v>
       </c>
-      <c r="J47" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="K47" s="12">
-        <v>0.30099999999999999</v>
-      </c>
-      <c r="L47" s="12">
-        <v>0</v>
-      </c>
-      <c r="M47" s="18">
+      <c r="J47">
+        <v>0.10038660000000001</v>
+      </c>
+      <c r="K47">
+        <v>0.30051480000000003</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
         <v>1</v>
       </c>
     </row>
@@ -35707,16 +35829,16 @@
       <c r="I48" s="31">
         <v>1</v>
       </c>
-      <c r="J48" s="12">
-        <v>6.2E-2</v>
-      </c>
-      <c r="K48" s="12">
-        <v>0.24</v>
-      </c>
-      <c r="L48" s="12">
-        <v>0</v>
-      </c>
-      <c r="M48" s="18">
+      <c r="J48">
+        <v>6.1550899999999999E-2</v>
+      </c>
+      <c r="K48">
+        <v>0.240338</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
         <v>1</v>
       </c>
     </row>
@@ -35748,16 +35870,16 @@
       <c r="I49" s="31">
         <v>1</v>
       </c>
-      <c r="J49" s="12">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="K49" s="12">
-        <v>0.30099999999999999</v>
-      </c>
-      <c r="L49" s="12">
-        <v>0</v>
-      </c>
-      <c r="M49" s="18">
+      <c r="J49">
+        <v>0.1010462</v>
+      </c>
+      <c r="K49">
+        <v>0.30138989999999999</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
         <v>1</v>
       </c>
     </row>
@@ -35789,16 +35911,16 @@
       <c r="I50" s="31">
         <v>1</v>
       </c>
-      <c r="J50" s="12">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="K50" s="12">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="L50" s="12">
-        <v>0</v>
-      </c>
-      <c r="M50" s="18">
+      <c r="J50">
+        <v>2.2375599999999999E-2</v>
+      </c>
+      <c r="K50">
+        <v>0.1479017</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
         <v>1</v>
       </c>
     </row>
@@ -35830,16 +35952,16 @@
       <c r="I51" s="31">
         <v>1</v>
       </c>
-      <c r="J51" s="12">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="K51" s="12">
-        <v>0.113</v>
-      </c>
-      <c r="L51" s="12">
-        <v>0</v>
-      </c>
-      <c r="M51" s="18">
+      <c r="J51">
+        <v>1.28249E-2</v>
+      </c>
+      <c r="K51">
+        <v>0.1125186</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
         <v>1</v>
       </c>
     </row>
@@ -35871,16 +35993,16 @@
       <c r="I52" s="31">
         <v>1</v>
       </c>
-      <c r="J52" s="12">
-        <v>0.114</v>
-      </c>
-      <c r="K52" s="12">
-        <v>0.318</v>
-      </c>
-      <c r="L52" s="12">
-        <v>0</v>
-      </c>
-      <c r="M52" s="18">
+      <c r="J52">
+        <v>0.11401210000000001</v>
+      </c>
+      <c r="K52">
+        <v>0.31782589999999999</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
         <v>1</v>
       </c>
     </row>
@@ -35912,16 +36034,16 @@
       <c r="I53" s="31">
         <v>1</v>
       </c>
-      <c r="J53" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="K53" s="12">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="L53" s="12">
-        <v>0</v>
-      </c>
-      <c r="M53" s="18">
+      <c r="J53">
+        <v>2.00082E-2</v>
+      </c>
+      <c r="K53">
+        <v>0.14002800000000001</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
         <v>1</v>
       </c>
     </row>
@@ -35953,16 +36075,16 @@
       <c r="I54" s="31">
         <v>1</v>
       </c>
-      <c r="J54" s="12">
-        <v>1.2E-2</v>
-      </c>
-      <c r="K54" s="12">
-        <v>0.11</v>
-      </c>
-      <c r="L54" s="12">
-        <v>0</v>
-      </c>
-      <c r="M54" s="18">
+      <c r="J54">
+        <v>1.22273E-2</v>
+      </c>
+      <c r="K54">
+        <v>0.1098991</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
         <v>1</v>
       </c>
     </row>
@@ -35994,16 +36116,16 @@
       <c r="I55" s="31">
         <v>1</v>
       </c>
-      <c r="J55" s="12">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="K55" s="12">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="L55" s="12">
-        <v>0</v>
-      </c>
-      <c r="M55" s="18">
+      <c r="J55">
+        <v>0.2076567</v>
+      </c>
+      <c r="K55">
+        <v>0.40562959999999998</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
         <v>1</v>
       </c>
     </row>
@@ -36035,16 +36157,16 @@
       <c r="I56" s="31">
         <v>1</v>
       </c>
-      <c r="J56" s="12">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="K56" s="12">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="L56" s="12">
-        <v>0</v>
-      </c>
-      <c r="M56" s="18">
+      <c r="J56">
+        <v>2.77478E-2</v>
+      </c>
+      <c r="K56">
+        <v>0.16424939999999999</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
         <v>1</v>
       </c>
     </row>
@@ -36076,16 +36198,16 @@
       <c r="I57" s="31">
         <v>1</v>
       </c>
-      <c r="J57" s="12">
-        <v>1.9E-2</v>
-      </c>
-      <c r="K57" s="12">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="L57" s="12">
-        <v>0</v>
-      </c>
-      <c r="M57" s="18">
+      <c r="J57">
+        <v>1.8577300000000001E-2</v>
+      </c>
+      <c r="K57">
+        <v>0.1350267</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
         <v>1</v>
       </c>
     </row>
@@ -36117,16 +36239,16 @@
       <c r="I58" s="31">
         <v>1</v>
       </c>
-      <c r="J58" s="12">
-        <v>5.5E-2</v>
-      </c>
-      <c r="K58" s="12">
-        <v>0.22800000000000001</v>
-      </c>
-      <c r="L58" s="12">
-        <v>0</v>
-      </c>
-      <c r="M58" s="18">
+      <c r="J58">
+        <v>5.4889300000000002E-2</v>
+      </c>
+      <c r="K58">
+        <v>0.2277641</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
         <v>1</v>
       </c>
     </row>
@@ -36158,16 +36280,16 @@
       <c r="I59" s="31">
         <v>1</v>
       </c>
-      <c r="J59" s="12">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K59" s="12">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="L59" s="12">
-        <v>0</v>
-      </c>
-      <c r="M59" s="18">
+      <c r="J59">
+        <v>6.5944000000000003E-3</v>
+      </c>
+      <c r="K59">
+        <v>8.0937599999999998E-2</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
         <v>1</v>
       </c>
     </row>
@@ -36199,16 +36321,16 @@
       <c r="I60" s="31">
         <v>1</v>
       </c>
-      <c r="J60" s="12">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="K60" s="12">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="L60" s="12">
-        <v>0</v>
-      </c>
-      <c r="M60" s="18">
+      <c r="J60">
+        <v>5.0972999999999999E-3</v>
+      </c>
+      <c r="K60">
+        <v>7.1213100000000001E-2</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
         <v>1</v>
       </c>
     </row>
@@ -36240,16 +36362,16 @@
       <c r="I61" s="31">
         <v>99835</v>
       </c>
-      <c r="J61" s="12">
-        <v>45485.923000000003</v>
-      </c>
-      <c r="K61" s="12">
+      <c r="J61">
+        <v>45485.919999999998</v>
+      </c>
+      <c r="K61">
         <v>27719.55</v>
       </c>
-      <c r="L61" s="12">
+      <c r="L61">
         <v>1001</v>
       </c>
-      <c r="M61" s="18">
+      <c r="M61">
         <v>99835</v>
       </c>
     </row>
@@ -36281,17 +36403,17 @@
       <c r="I62" s="31">
         <v>1323.4</v>
       </c>
-      <c r="J62" s="12">
-        <v>813.86199999999997</v>
-      </c>
-      <c r="K62" s="12">
-        <v>82.254000000000005</v>
-      </c>
-      <c r="L62" s="12">
-        <v>466</v>
-      </c>
-      <c r="M62" s="18">
-        <v>1323</v>
+      <c r="J62">
+        <v>813.86159999999995</v>
+      </c>
+      <c r="K62">
+        <v>82.254450000000006</v>
+      </c>
+      <c r="L62">
+        <v>465.95</v>
+      </c>
+      <c r="M62">
+        <v>1323.4</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -36322,16 +36444,16 @@
       <c r="I63" s="31">
         <v>1</v>
       </c>
-      <c r="J63" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="K63" s="12">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="L63" s="12">
-        <v>0</v>
-      </c>
-      <c r="M63" s="18">
+      <c r="J63">
+        <v>2.0498300000000001E-2</v>
+      </c>
+      <c r="K63">
+        <v>0.1416973</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63">
         <v>1</v>
       </c>
     </row>
@@ -36363,16 +36485,16 @@
       <c r="I64" s="31">
         <v>1</v>
       </c>
-      <c r="J64" s="12">
-        <v>0.99199999999999999</v>
-      </c>
-      <c r="K64" s="12">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="L64" s="12">
-        <v>0</v>
-      </c>
-      <c r="M64" s="18">
+      <c r="J64">
+        <v>0.99249399999999999</v>
+      </c>
+      <c r="K64">
+        <v>6.1484700000000003E-2</v>
+      </c>
+      <c r="L64">
+        <v>8.3333299999999999E-2</v>
+      </c>
+      <c r="M64">
         <v>1</v>
       </c>
     </row>
@@ -36404,16 +36526,16 @@
       <c r="I65" s="31">
         <v>1</v>
       </c>
-      <c r="J65" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="K65" s="12">
-        <v>2.7E-2</v>
-      </c>
-      <c r="L65" s="12">
-        <v>0</v>
-      </c>
-      <c r="M65" s="18">
+      <c r="J65">
+        <v>7.3470000000000002E-4</v>
+      </c>
+      <c r="K65">
+        <v>2.7094900000000002E-2</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
         <v>1</v>
       </c>
     </row>
@@ -36445,16 +36567,16 @@
       <c r="I66" s="31">
         <v>1</v>
       </c>
-      <c r="J66" s="12">
-        <v>0.115</v>
-      </c>
-      <c r="K66" s="12">
-        <v>0.31900000000000001</v>
-      </c>
-      <c r="L66" s="12">
-        <v>0</v>
-      </c>
-      <c r="M66" s="18">
+      <c r="J66">
+        <v>0.1153762</v>
+      </c>
+      <c r="K66">
+        <v>0.31947540000000002</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
         <v>1</v>
       </c>
     </row>
@@ -36486,16 +36608,16 @@
       <c r="I67" s="31">
         <v>1</v>
       </c>
-      <c r="J67" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="K67" s="12">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="L67" s="12">
-        <v>0</v>
-      </c>
-      <c r="M67" s="18">
+      <c r="J67">
+        <v>9.7634000000000002E-3</v>
+      </c>
+      <c r="K67">
+        <v>9.8326399999999994E-2</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+      <c r="M67">
         <v>1</v>
       </c>
     </row>
@@ -36527,16 +36649,16 @@
       <c r="I68" s="31">
         <v>1</v>
       </c>
-      <c r="J68" s="12">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="K68" s="12">
-        <v>0.23300000000000001</v>
-      </c>
-      <c r="L68" s="12">
-        <v>0</v>
-      </c>
-      <c r="M68" s="18">
+      <c r="J68">
+        <v>5.7606299999999999E-2</v>
+      </c>
+      <c r="K68">
+        <v>0.2329975</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
         <v>1</v>
       </c>
     </row>
@@ -36568,16 +36690,16 @@
       <c r="I69" s="31">
         <v>1</v>
       </c>
-      <c r="J69" s="12">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="K69" s="12">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="L69" s="12">
-        <v>0</v>
-      </c>
-      <c r="M69" s="18">
+      <c r="J69">
+        <v>4.3558100000000002E-2</v>
+      </c>
+      <c r="K69">
+        <v>0.20410990000000001</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
         <v>1</v>
       </c>
     </row>
@@ -36609,16 +36731,16 @@
       <c r="I70" s="31">
         <v>1</v>
       </c>
-      <c r="J70" s="12">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="K70" s="12">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="L70" s="12">
-        <v>0</v>
-      </c>
-      <c r="M70" s="18">
+      <c r="J70">
+        <v>3.2818300000000002E-2</v>
+      </c>
+      <c r="K70">
+        <v>0.17816070000000001</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
         <v>1</v>
       </c>
     </row>
@@ -36650,16 +36772,16 @@
       <c r="I71" s="31">
         <v>1</v>
       </c>
-      <c r="J71" s="12">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="K71" s="12">
-        <v>0.254</v>
-      </c>
-      <c r="L71" s="12">
-        <v>0</v>
-      </c>
-      <c r="M71" s="18">
+      <c r="J71">
+        <v>6.9326200000000004E-2</v>
+      </c>
+      <c r="K71">
+        <v>0.25400800000000001</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
         <v>1</v>
       </c>
     </row>
@@ -36691,16 +36813,16 @@
       <c r="I72" s="31">
         <v>1</v>
       </c>
-      <c r="J72" s="12">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="K72" s="12">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="L72" s="12">
-        <v>0</v>
-      </c>
-      <c r="M72" s="18">
+      <c r="J72">
+        <v>3.2183400000000001E-2</v>
+      </c>
+      <c r="K72">
+        <v>0.1764868</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
         <v>1</v>
       </c>
     </row>
@@ -36732,16 +36854,16 @@
       <c r="I73" s="31">
         <v>1</v>
       </c>
-      <c r="J73" s="12">
-        <v>0.06</v>
-      </c>
-      <c r="K73" s="12">
-        <v>0.23699999999999999</v>
-      </c>
-      <c r="L73" s="12">
-        <v>0</v>
-      </c>
-      <c r="M73" s="18">
+      <c r="J73">
+        <v>6.00037E-2</v>
+      </c>
+      <c r="K73">
+        <v>0.2374937</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
         <v>1</v>
       </c>
     </row>
@@ -36773,16 +36895,16 @@
       <c r="I74" s="31">
         <v>1</v>
       </c>
-      <c r="J74" s="12">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="K74" s="12">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="L74" s="12">
-        <v>0</v>
-      </c>
-      <c r="M74" s="18">
+      <c r="J74">
+        <v>4.3334999999999997E-3</v>
+      </c>
+      <c r="K74">
+        <v>6.5686300000000003E-2</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
         <v>1</v>
       </c>
     </row>
@@ -36814,16 +36936,16 @@
       <c r="I75" s="31">
         <v>1</v>
       </c>
-      <c r="J75" s="12">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="K75" s="12">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="L75" s="12">
-        <v>0</v>
-      </c>
-      <c r="M75" s="18">
+      <c r="J75">
+        <v>1.0732999999999999E-2</v>
+      </c>
+      <c r="K75">
+        <v>0.1030426</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
         <v>1</v>
       </c>
     </row>
@@ -36855,16 +36977,16 @@
       <c r="I76" s="31">
         <v>1</v>
       </c>
-      <c r="J76" s="12">
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="K76" s="12">
-        <v>0.45200000000000001</v>
-      </c>
-      <c r="L76" s="12">
-        <v>0</v>
-      </c>
-      <c r="M76" s="18">
+      <c r="J76">
+        <v>0.28550550000000002</v>
+      </c>
+      <c r="K76">
+        <v>0.45165490000000003</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
         <v>1</v>
       </c>
     </row>
@@ -36896,16 +37018,16 @@
       <c r="I77" s="31">
         <v>1</v>
       </c>
-      <c r="J77" s="12">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="K77" s="12">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="L77" s="12">
-        <v>0</v>
-      </c>
-      <c r="M77" s="18">
+      <c r="J77">
+        <v>9.5277100000000003E-2</v>
+      </c>
+      <c r="K77">
+        <v>0.29359740000000001</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
         <v>1</v>
       </c>
     </row>
@@ -36937,16 +37059,16 @@
       <c r="I78" s="31">
         <v>1</v>
       </c>
-      <c r="J78" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="K78" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="L78" s="12">
-        <v>0</v>
-      </c>
-      <c r="M78" s="18">
+      <c r="J78">
+        <v>1.0198799999999999E-2</v>
+      </c>
+      <c r="K78">
+        <v>0.1004726</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
         <v>1</v>
       </c>
     </row>
@@ -36978,16 +37100,16 @@
       <c r="I79" s="31">
         <v>1</v>
       </c>
-      <c r="J79" s="12">
-        <v>1.2E-2</v>
-      </c>
-      <c r="K79" s="12">
-        <v>0.108</v>
-      </c>
-      <c r="L79" s="12">
-        <v>0</v>
-      </c>
-      <c r="M79" s="18">
+      <c r="J79">
+        <v>1.18458E-2</v>
+      </c>
+      <c r="K79">
+        <v>0.10819189999999999</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
         <v>1</v>
       </c>
     </row>
@@ -37019,16 +37141,16 @@
       <c r="I80" s="31">
         <v>1</v>
       </c>
-      <c r="J80" s="12">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="K80" s="12">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="L80" s="12">
-        <v>0</v>
-      </c>
-      <c r="M80" s="18">
+      <c r="J80">
+        <v>3.7008000000000002E-3</v>
+      </c>
+      <c r="K80">
+        <v>6.0721499999999998E-2</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80">
         <v>1</v>
       </c>
     </row>
@@ -37060,16 +37182,16 @@
       <c r="I81" s="31">
         <v>1</v>
       </c>
-      <c r="J81" s="12">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="K81" s="12">
-        <v>0.25800000000000001</v>
-      </c>
-      <c r="L81" s="12">
-        <v>0</v>
-      </c>
-      <c r="M81" s="18">
+      <c r="J81">
+        <v>7.1451200000000006E-2</v>
+      </c>
+      <c r="K81">
+        <v>0.2575771</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81">
         <v>1</v>
       </c>
     </row>
@@ -37101,16 +37223,16 @@
       <c r="I82" s="31">
         <v>1</v>
       </c>
-      <c r="J82" s="12">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="K82" s="12">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="L82" s="12">
-        <v>0</v>
-      </c>
-      <c r="M82" s="18">
+      <c r="J82">
+        <v>2.8124099999999999E-2</v>
+      </c>
+      <c r="K82">
+        <v>0.16532740000000001</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
         <v>1</v>
       </c>
     </row>
@@ -37142,16 +37264,16 @@
       <c r="I83" s="31">
         <v>1</v>
       </c>
-      <c r="J83" s="12">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="K83" s="12">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="L83" s="12">
-        <v>0</v>
-      </c>
-      <c r="M83" s="18">
+      <c r="J83">
+        <v>9.0606999999999997E-3</v>
+      </c>
+      <c r="K83">
+        <v>9.4755599999999995E-2</v>
+      </c>
+      <c r="L83">
+        <v>0</v>
+      </c>
+      <c r="M83">
         <v>1</v>
       </c>
     </row>
@@ -37183,16 +37305,16 @@
       <c r="I84" s="31">
         <v>1</v>
       </c>
-      <c r="J84" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="K84" s="12">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="L84" s="12">
-        <v>0</v>
-      </c>
-      <c r="M84" s="18">
+      <c r="J84">
+        <v>2.0247899999999999E-2</v>
+      </c>
+      <c r="K84">
+        <v>0.140847</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84">
         <v>1</v>
       </c>
     </row>
@@ -37224,16 +37346,16 @@
       <c r="I85" s="31">
         <v>1</v>
       </c>
-      <c r="J85" s="12">
-        <v>3.9E-2</v>
-      </c>
-      <c r="K85" s="12">
-        <v>0.192</v>
-      </c>
-      <c r="L85" s="12">
-        <v>0</v>
-      </c>
-      <c r="M85" s="18">
+      <c r="J85">
+        <v>3.8533900000000003E-2</v>
+      </c>
+      <c r="K85">
+        <v>0.19248129999999999</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85">
         <v>1</v>
       </c>
     </row>
@@ -37265,16 +37387,16 @@
       <c r="I86" s="31">
         <v>1</v>
       </c>
-      <c r="J86" s="12">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="K86" s="12">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="L86" s="12">
-        <v>0</v>
-      </c>
-      <c r="M86" s="18">
+      <c r="J86">
+        <v>3.1917999999999998E-3</v>
+      </c>
+      <c r="K86">
+        <v>5.64056E-2</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86">
         <v>1</v>
       </c>
     </row>
@@ -37306,16 +37428,16 @@
       <c r="I87" s="31">
         <v>1</v>
       </c>
-      <c r="J87" s="12">
-        <v>2E-3</v>
-      </c>
-      <c r="K87" s="12">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="L87" s="12">
-        <v>0</v>
-      </c>
-      <c r="M87" s="18">
+      <c r="J87">
+        <v>2.0996999999999999E-3</v>
+      </c>
+      <c r="K87">
+        <v>4.5774099999999998E-2</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87">
         <v>1</v>
       </c>
     </row>
@@ -37347,16 +37469,16 @@
       <c r="I88" s="31">
         <v>1</v>
       </c>
-      <c r="J88" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="K88" s="12">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="L88" s="12">
-        <v>0</v>
-      </c>
-      <c r="M88" s="18">
+      <c r="J88">
+        <v>1.8436999999999999E-2</v>
+      </c>
+      <c r="K88">
+        <v>0.13452549999999999</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88">
         <v>1</v>
       </c>
     </row>
@@ -37388,16 +37510,16 @@
       <c r="I89" s="31">
         <v>1</v>
       </c>
-      <c r="J89" s="12">
-        <v>1.2E-2</v>
-      </c>
-      <c r="K89" s="12">
-        <v>0.11</v>
-      </c>
-      <c r="L89" s="12">
-        <v>0</v>
-      </c>
-      <c r="M89" s="18">
+      <c r="J89">
+        <v>1.21663E-2</v>
+      </c>
+      <c r="K89">
+        <v>0.10962810000000001</v>
+      </c>
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89">
         <v>1</v>
       </c>
     </row>
@@ -37429,16 +37551,16 @@
       <c r="I90" s="31">
         <v>1</v>
       </c>
-      <c r="J90" s="12">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K90" s="12">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="L90" s="12">
-        <v>0</v>
-      </c>
-      <c r="M90" s="18">
+      <c r="J90">
+        <v>6.7403000000000003E-3</v>
+      </c>
+      <c r="K90">
+        <v>8.1822000000000006E-2</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90">
         <v>1</v>
       </c>
     </row>
@@ -37470,16 +37592,16 @@
       <c r="I91" s="31">
         <v>1</v>
       </c>
-      <c r="J91" s="12">
-        <v>2.4E-2</v>
-      </c>
-      <c r="K91" s="12">
-        <v>0.154</v>
-      </c>
-      <c r="L91" s="12">
-        <v>0</v>
-      </c>
-      <c r="M91" s="18">
+      <c r="J91">
+        <v>2.42495E-2</v>
+      </c>
+      <c r="K91">
+        <v>0.15382280000000001</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+      <c r="M91">
         <v>1</v>
       </c>
     </row>
@@ -37511,16 +37633,16 @@
       <c r="I92" s="31">
         <v>1</v>
       </c>
-      <c r="J92" s="12">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="K92" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="L92" s="12">
-        <v>0</v>
-      </c>
-      <c r="M92" s="18">
+      <c r="J92">
+        <v>2.5378000000000002E-3</v>
+      </c>
+      <c r="K92">
+        <v>5.03124E-2</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92">
         <v>1</v>
       </c>
     </row>
@@ -37552,16 +37674,16 @@
       <c r="I93" s="31">
         <v>1</v>
       </c>
-      <c r="J93" s="12">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="K93" s="12">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="L93" s="12">
-        <v>0</v>
-      </c>
-      <c r="M93" s="18">
+      <c r="J93">
+        <v>3.4188999999999999E-3</v>
+      </c>
+      <c r="K93">
+        <v>5.8370900000000003E-2</v>
+      </c>
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93">
         <v>1</v>
       </c>
     </row>
@@ -37593,16 +37715,16 @@
       <c r="I94" s="31">
         <v>1</v>
       </c>
-      <c r="J94" s="12">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="K94" s="12">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="L94" s="12">
-        <v>0</v>
-      </c>
-      <c r="M94" s="18">
+      <c r="J94">
+        <v>4.6512000000000003E-3</v>
+      </c>
+      <c r="K94">
+        <v>6.8040699999999996E-2</v>
+      </c>
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94">
         <v>1</v>
       </c>
     </row>
@@ -37634,16 +37756,16 @@
       <c r="I95" s="31">
         <v>1</v>
       </c>
-      <c r="J95" s="12">
-        <v>0</v>
-      </c>
-      <c r="K95" s="12">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="L95" s="12">
-        <v>0</v>
-      </c>
-      <c r="M95" s="18">
+      <c r="J95">
+        <v>3.055E-4</v>
+      </c>
+      <c r="K95">
+        <v>1.7476200000000001E-2</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95">
         <v>1</v>
       </c>
     </row>
@@ -37675,16 +37797,16 @@
       <c r="I96" s="31">
         <v>1</v>
       </c>
-      <c r="J96" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="K96" s="12">
-        <v>0.218</v>
-      </c>
-      <c r="L96" s="12">
-        <v>0</v>
-      </c>
-      <c r="M96" s="18">
+      <c r="J96">
+        <v>5.0218400000000003E-2</v>
+      </c>
+      <c r="K96">
+        <v>0.21839520000000001</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96">
         <v>1</v>
       </c>
     </row>
@@ -37716,16 +37838,16 @@
       <c r="I97" s="31">
         <v>1</v>
       </c>
-      <c r="J97" s="12">
-        <v>2E-3</v>
-      </c>
-      <c r="K97" s="12">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="L97" s="12">
-        <v>0</v>
-      </c>
-      <c r="M97" s="18">
+      <c r="J97">
+        <v>2.3701999999999998E-3</v>
+      </c>
+      <c r="K97">
+        <v>4.8627299999999998E-2</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97">
         <v>1</v>
       </c>
     </row>
@@ -37757,16 +37879,16 @@
       <c r="I98" s="31">
         <v>1</v>
       </c>
-      <c r="J98" s="12">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="K98" s="12">
-        <v>0.156</v>
-      </c>
-      <c r="L98" s="12">
-        <v>0</v>
-      </c>
-      <c r="M98" s="18">
+      <c r="J98">
+        <v>2.4908099999999999E-2</v>
+      </c>
+      <c r="K98">
+        <v>0.15584500000000001</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98">
         <v>1</v>
       </c>
     </row>
@@ -37798,16 +37920,16 @@
       <c r="I99" s="31">
         <v>1</v>
       </c>
-      <c r="J99" s="12">
-        <v>0.04</v>
-      </c>
-      <c r="K99" s="12">
-        <v>0.19600000000000001</v>
-      </c>
-      <c r="L99" s="12">
-        <v>0</v>
-      </c>
-      <c r="M99" s="18">
+      <c r="J99">
+        <v>4.0026800000000001E-2</v>
+      </c>
+      <c r="K99">
+        <v>0.1960221</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99">
         <v>1</v>
       </c>
     </row>
@@ -37839,16 +37961,16 @@
       <c r="I100" s="31">
         <v>1</v>
       </c>
-      <c r="J100" s="12">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="K100" s="12">
-        <v>0.105</v>
-      </c>
-      <c r="L100" s="12">
-        <v>0</v>
-      </c>
-      <c r="M100" s="18">
+      <c r="J100">
+        <v>1.1044399999999999E-2</v>
+      </c>
+      <c r="K100">
+        <v>0.1045103</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100">
         <v>1</v>
       </c>
     </row>
@@ -37880,16 +38002,16 @@
       <c r="I101" s="31">
         <v>1</v>
       </c>
-      <c r="J101" s="12">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K101" s="12">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="L101" s="12">
-        <v>0</v>
-      </c>
-      <c r="M101" s="18">
+      <c r="J101">
+        <v>6.6042000000000002E-3</v>
+      </c>
+      <c r="K101">
+        <v>8.0997600000000003E-2</v>
+      </c>
+      <c r="L101">
+        <v>0</v>
+      </c>
+      <c r="M101">
         <v>1</v>
       </c>
     </row>
@@ -37921,16 +38043,16 @@
       <c r="I102" s="31">
         <v>1</v>
       </c>
-      <c r="J102" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="K102" s="12">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="L102" s="12">
-        <v>0</v>
-      </c>
-      <c r="M102" s="18">
+      <c r="J102">
+        <v>1.2918000000000001E-3</v>
+      </c>
+      <c r="K102">
+        <v>3.5919100000000002E-2</v>
+      </c>
+      <c r="L102">
+        <v>0</v>
+      </c>
+      <c r="M102">
         <v>1</v>
       </c>
     </row>
@@ -37962,16 +38084,16 @@
       <c r="I103" s="31">
         <v>1</v>
       </c>
-      <c r="J103" s="12">
-        <v>0.18</v>
-      </c>
-      <c r="K103" s="12">
-        <v>0.38400000000000001</v>
-      </c>
-      <c r="L103" s="12">
-        <v>0</v>
-      </c>
-      <c r="M103" s="18">
+      <c r="J103">
+        <v>0.17998549999999999</v>
+      </c>
+      <c r="K103">
+        <v>0.3841754</v>
+      </c>
+      <c r="L103">
+        <v>0</v>
+      </c>
+      <c r="M103">
         <v>1</v>
       </c>
     </row>
@@ -38003,16 +38125,16 @@
       <c r="I104" s="31">
         <v>1</v>
       </c>
-      <c r="J104" s="12">
-        <v>0.33800000000000002</v>
-      </c>
-      <c r="K104" s="12">
-        <v>0.47299999999999998</v>
-      </c>
-      <c r="L104" s="12">
-        <v>0</v>
-      </c>
-      <c r="M104" s="18">
+      <c r="J104">
+        <v>0.33814129999999998</v>
+      </c>
+      <c r="K104">
+        <v>0.47307690000000002</v>
+      </c>
+      <c r="L104">
+        <v>0</v>
+      </c>
+      <c r="M104">
         <v>1</v>
       </c>
     </row>
@@ -38044,16 +38166,16 @@
       <c r="I105" s="31">
         <v>1</v>
       </c>
-      <c r="J105" s="12">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="K105" s="12">
-        <v>0.27400000000000002</v>
-      </c>
-      <c r="L105" s="12">
-        <v>0</v>
-      </c>
-      <c r="M105" s="18">
+      <c r="J105">
+        <v>8.1986900000000001E-2</v>
+      </c>
+      <c r="K105">
+        <v>0.2743448</v>
+      </c>
+      <c r="L105">
+        <v>0</v>
+      </c>
+      <c r="M105">
         <v>1</v>
       </c>
     </row>
@@ -38085,16 +38207,16 @@
       <c r="I106" s="31">
         <v>1</v>
       </c>
-      <c r="J106" s="12">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="K106" s="12">
-        <v>0.214</v>
-      </c>
-      <c r="L106" s="12">
-        <v>0</v>
-      </c>
-      <c r="M106" s="18">
+      <c r="J106">
+        <v>4.8317699999999998E-2</v>
+      </c>
+      <c r="K106">
+        <v>0.21443680000000001</v>
+      </c>
+      <c r="L106">
+        <v>0</v>
+      </c>
+      <c r="M106">
         <v>1</v>
       </c>
     </row>
@@ -38126,16 +38248,16 @@
       <c r="I107" s="31">
         <v>1</v>
       </c>
-      <c r="J107" s="12">
-        <v>0.107</v>
-      </c>
-      <c r="K107" s="12">
-        <v>0.309</v>
-      </c>
-      <c r="L107" s="12">
-        <v>0</v>
-      </c>
-      <c r="M107" s="18">
+      <c r="J107">
+        <v>0.1067512</v>
+      </c>
+      <c r="K107">
+        <v>0.30879669999999998</v>
+      </c>
+      <c r="L107">
+        <v>0</v>
+      </c>
+      <c r="M107">
         <v>1</v>
       </c>
     </row>
@@ -38167,16 +38289,16 @@
       <c r="I108" s="31">
         <v>1</v>
       </c>
-      <c r="J108" s="12">
-        <v>0.30199999999999999</v>
-      </c>
-      <c r="K108" s="12">
-        <v>0.45900000000000002</v>
-      </c>
-      <c r="L108" s="12">
-        <v>0</v>
-      </c>
-      <c r="M108" s="18">
+      <c r="J108">
+        <v>0.30170609999999998</v>
+      </c>
+      <c r="K108">
+        <v>0.45899839999999997</v>
+      </c>
+      <c r="L108">
+        <v>0</v>
+      </c>
+      <c r="M108">
         <v>1</v>
       </c>
     </row>
@@ -38208,16 +38330,16 @@
       <c r="I109" s="31">
         <v>1</v>
       </c>
-      <c r="J109" s="12">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="K109" s="12">
-        <v>0.115</v>
-      </c>
-      <c r="L109" s="12">
-        <v>0</v>
-      </c>
-      <c r="M109" s="18">
+      <c r="J109">
+        <v>1.34631E-2</v>
+      </c>
+      <c r="K109">
+        <v>0.1152468</v>
+      </c>
+      <c r="L109">
+        <v>0</v>
+      </c>
+      <c r="M109">
         <v>1</v>
       </c>
     </row>
@@ -38249,16 +38371,16 @@
       <c r="I110" s="31">
         <v>1</v>
       </c>
-      <c r="J110" s="12">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="K110" s="12">
-        <v>0.219</v>
-      </c>
-      <c r="L110" s="12">
-        <v>0</v>
-      </c>
-      <c r="M110" s="18">
+      <c r="J110">
+        <v>5.0697699999999998E-2</v>
+      </c>
+      <c r="K110">
+        <v>0.21937970000000001</v>
+      </c>
+      <c r="L110">
+        <v>0</v>
+      </c>
+      <c r="M110">
         <v>1</v>
       </c>
     </row>
@@ -38290,16 +38412,16 @@
       <c r="I111" s="31">
         <v>1</v>
       </c>
-      <c r="J111" s="12">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="K111" s="12">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="L111" s="12">
-        <v>0</v>
-      </c>
-      <c r="M111" s="18">
+      <c r="J111">
+        <v>4.4818700000000003E-2</v>
+      </c>
+      <c r="K111">
+        <v>0.2069058</v>
+      </c>
+      <c r="L111">
+        <v>0</v>
+      </c>
+      <c r="M111">
         <v>1</v>
       </c>
     </row>
@@ -38331,16 +38453,16 @@
       <c r="I112" s="31">
         <v>1</v>
       </c>
-      <c r="J112" s="12">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="K112" s="12">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="L112" s="12">
-        <v>0</v>
-      </c>
-      <c r="M112" s="18">
+      <c r="J112">
+        <v>2.9383E-3</v>
+      </c>
+      <c r="K112">
+        <v>5.4126300000000002E-2</v>
+      </c>
+      <c r="L112">
+        <v>0</v>
+      </c>
+      <c r="M112">
         <v>1</v>
       </c>
     </row>
@@ -38372,16 +38494,16 @@
       <c r="I113" s="31">
         <v>1</v>
       </c>
-      <c r="J113" s="12">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="K113" s="12">
-        <v>0.23300000000000001</v>
-      </c>
-      <c r="L113" s="12">
-        <v>0</v>
-      </c>
-      <c r="M113" s="18">
+      <c r="J113">
+        <v>5.7437000000000002E-2</v>
+      </c>
+      <c r="K113">
+        <v>0.23267570000000001</v>
+      </c>
+      <c r="L113">
+        <v>0</v>
+      </c>
+      <c r="M113">
         <v>1</v>
       </c>
     </row>
@@ -38413,16 +38535,16 @@
       <c r="I114" s="31">
         <v>1</v>
       </c>
-      <c r="J114" s="12">
-        <v>0.16</v>
-      </c>
-      <c r="K114" s="12">
-        <v>0.36699999999999999</v>
-      </c>
-      <c r="L114" s="12">
-        <v>0</v>
-      </c>
-      <c r="M114" s="18">
+      <c r="J114">
+        <v>0.16046820000000001</v>
+      </c>
+      <c r="K114">
+        <v>0.36703970000000002</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+      <c r="M114">
         <v>1</v>
       </c>
     </row>
@@ -38454,16 +38576,16 @@
       <c r="I115" s="31">
         <v>1</v>
       </c>
-      <c r="J115" s="12">
-        <v>0</v>
-      </c>
-      <c r="K115" s="12">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="L115" s="12">
-        <v>0</v>
-      </c>
-      <c r="M115" s="18">
+      <c r="J115">
+        <v>4.0899999999999998E-5</v>
+      </c>
+      <c r="K115">
+        <v>6.3987000000000002E-3</v>
+      </c>
+      <c r="L115">
+        <v>0</v>
+      </c>
+      <c r="M115">
         <v>1</v>
       </c>
     </row>
@@ -38495,16 +38617,16 @@
       <c r="I116" s="31">
         <v>1</v>
       </c>
-      <c r="J116" s="12">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="K116" s="12">
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="L116" s="12">
-        <v>0</v>
-      </c>
-      <c r="M116" s="18">
+      <c r="J116">
+        <v>0.27217649999999999</v>
+      </c>
+      <c r="K116">
+        <v>0.44508029999999998</v>
+      </c>
+      <c r="L116">
+        <v>0</v>
+      </c>
+      <c r="M116">
         <v>1</v>
       </c>
     </row>
@@ -38536,16 +38658,16 @@
       <c r="I117" s="31">
         <v>1</v>
       </c>
-      <c r="J117" s="12">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="K117" s="12">
-        <v>0.251</v>
-      </c>
-      <c r="L117" s="12">
-        <v>0</v>
-      </c>
-      <c r="M117" s="18">
+      <c r="J117">
+        <v>6.7772899999999997E-2</v>
+      </c>
+      <c r="K117">
+        <v>0.25135580000000002</v>
+      </c>
+      <c r="L117">
+        <v>0</v>
+      </c>
+      <c r="M117">
         <v>1</v>
       </c>
     </row>
@@ -38577,16 +38699,16 @@
       <c r="I118" s="31">
         <v>1</v>
       </c>
-      <c r="J118" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="K118" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="L118" s="12">
-        <v>0</v>
-      </c>
-      <c r="M118" s="18">
+      <c r="J118">
+        <v>1.0152700000000001E-2</v>
+      </c>
+      <c r="K118">
+        <v>0.100248</v>
+      </c>
+      <c r="L118">
+        <v>0</v>
+      </c>
+      <c r="M118">
         <v>1</v>
       </c>
     </row>
@@ -38618,16 +38740,16 @@
       <c r="I119" s="31">
         <v>1</v>
       </c>
-      <c r="J119" s="12">
-        <v>0</v>
-      </c>
-      <c r="K119" s="12">
-        <v>1.6E-2</v>
-      </c>
-      <c r="L119" s="12">
-        <v>0</v>
-      </c>
-      <c r="M119" s="18">
+      <c r="J119">
+        <v>2.4640000000000003E-4</v>
+      </c>
+      <c r="K119">
+        <v>1.56946E-2</v>
+      </c>
+      <c r="L119">
+        <v>0</v>
+      </c>
+      <c r="M119">
         <v>1</v>
       </c>
     </row>
@@ -38659,16 +38781,16 @@
       <c r="I120" s="31">
         <v>1</v>
       </c>
-      <c r="J120" s="12">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="K120" s="12">
-        <v>0.128</v>
-      </c>
-      <c r="L120" s="12">
-        <v>0</v>
-      </c>
-      <c r="M120" s="18">
+      <c r="J120">
+        <v>1.6606300000000001E-2</v>
+      </c>
+      <c r="K120">
+        <v>0.12779090000000001</v>
+      </c>
+      <c r="L120">
+        <v>0</v>
+      </c>
+      <c r="M120">
         <v>1</v>
       </c>
     </row>
@@ -38700,16 +38822,16 @@
       <c r="I121" s="31">
         <v>1</v>
       </c>
-      <c r="J121" s="12">
-        <v>0.30299999999999999</v>
-      </c>
-      <c r="K121" s="12">
-        <v>0.46</v>
-      </c>
-      <c r="L121" s="12">
-        <v>0</v>
-      </c>
-      <c r="M121" s="18">
+      <c r="J121">
+        <v>0.3032627</v>
+      </c>
+      <c r="K121">
+        <v>0.45966780000000002</v>
+      </c>
+      <c r="L121">
+        <v>0</v>
+      </c>
+      <c r="M121">
         <v>1</v>
       </c>
     </row>
@@ -38741,16 +38863,16 @@
       <c r="I122" s="31">
         <v>1</v>
       </c>
-      <c r="J122" s="12">
-        <v>1.4E-2</v>
-      </c>
-      <c r="K122" s="12">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="L122" s="12">
-        <v>0</v>
-      </c>
-      <c r="M122" s="18">
+      <c r="J122">
+        <v>1.37825E-2</v>
+      </c>
+      <c r="K122">
+        <v>0.1165871</v>
+      </c>
+      <c r="L122">
+        <v>0</v>
+      </c>
+      <c r="M122">
         <v>1</v>
       </c>
     </row>
@@ -38782,16 +38904,16 @@
       <c r="I123" s="31">
         <v>1</v>
       </c>
-      <c r="J123" s="12">
-        <v>6.3E-2</v>
-      </c>
-      <c r="K123" s="12">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="L123" s="12">
-        <v>0</v>
-      </c>
-      <c r="M123" s="18">
+      <c r="J123">
+        <v>6.3013799999999995E-2</v>
+      </c>
+      <c r="K123">
+        <v>0.2429878</v>
+      </c>
+      <c r="L123">
+        <v>0</v>
+      </c>
+      <c r="M123">
         <v>1</v>
       </c>
     </row>
@@ -38823,16 +38945,16 @@
       <c r="I124" s="31">
         <v>1</v>
       </c>
-      <c r="J124" s="12">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="K124" s="12">
-        <v>0.188</v>
-      </c>
-      <c r="L124" s="12">
-        <v>0</v>
-      </c>
-      <c r="M124" s="18">
+      <c r="J124">
+        <v>3.68893E-2</v>
+      </c>
+      <c r="K124">
+        <v>0.18848999999999999</v>
+      </c>
+      <c r="L124">
+        <v>0</v>
+      </c>
+      <c r="M124">
         <v>1</v>
       </c>
     </row>
@@ -38864,16 +38986,16 @@
       <c r="I125" s="31">
         <v>1</v>
       </c>
-      <c r="J125" s="12">
-        <v>0</v>
-      </c>
-      <c r="K125" s="12">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="L125" s="12">
-        <v>0</v>
-      </c>
-      <c r="M125" s="18">
+      <c r="J125">
+        <v>6.4999999999999994E-5</v>
+      </c>
+      <c r="K125">
+        <v>8.0634999999999995E-3</v>
+      </c>
+      <c r="L125">
+        <v>0</v>
+      </c>
+      <c r="M125">
         <v>1</v>
       </c>
     </row>
@@ -38905,16 +39027,16 @@
       <c r="I126" s="31">
         <v>1</v>
       </c>
-      <c r="J126" s="12">
-        <v>0</v>
-      </c>
-      <c r="K126" s="12">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="L126" s="12">
-        <v>0</v>
-      </c>
-      <c r="M126" s="18">
+      <c r="J126">
+        <v>4.9470000000000004E-4</v>
+      </c>
+      <c r="K126">
+        <v>2.2236200000000001E-2</v>
+      </c>
+      <c r="L126">
+        <v>0</v>
+      </c>
+      <c r="M126">
         <v>1</v>
       </c>
     </row>
@@ -38946,16 +39068,16 @@
       <c r="I127" s="31">
         <v>1</v>
       </c>
-      <c r="J127" s="12">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="K127" s="12">
-        <v>0.113</v>
-      </c>
-      <c r="L127" s="12">
-        <v>0</v>
-      </c>
-      <c r="M127" s="18">
+      <c r="J127">
+        <v>1.28472E-2</v>
+      </c>
+      <c r="K127">
+        <v>0.1126149</v>
+      </c>
+      <c r="L127">
+        <v>0</v>
+      </c>
+      <c r="M127">
         <v>1</v>
       </c>
     </row>
@@ -38987,16 +39109,16 @@
       <c r="I128" s="31">
         <v>1</v>
       </c>
-      <c r="J128" s="12">
-        <v>3.1E-2</v>
-      </c>
-      <c r="K128" s="12">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="L128" s="12">
-        <v>0</v>
-      </c>
-      <c r="M128" s="18">
+      <c r="J128">
+        <v>3.0817199999999999E-2</v>
+      </c>
+      <c r="K128">
+        <v>0.17282230000000001</v>
+      </c>
+      <c r="L128">
+        <v>0</v>
+      </c>
+      <c r="M128">
         <v>1</v>
       </c>
     </row>
@@ -39028,16 +39150,16 @@
       <c r="I129" s="31">
         <v>1</v>
       </c>
-      <c r="J129" s="12">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="K129" s="12">
-        <v>0.224</v>
-      </c>
-      <c r="L129" s="12">
-        <v>0</v>
-      </c>
-      <c r="M129" s="18">
+      <c r="J129">
+        <v>5.2833999999999999E-2</v>
+      </c>
+      <c r="K129">
+        <v>0.22370190000000001</v>
+      </c>
+      <c r="L129">
+        <v>0</v>
+      </c>
+      <c r="M129">
         <v>1</v>
       </c>
     </row>
@@ -39069,16 +39191,16 @@
       <c r="I130" s="31">
         <v>1</v>
       </c>
-      <c r="J130" s="12">
-        <v>0</v>
-      </c>
-      <c r="K130" s="12">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="L130" s="12">
-        <v>0</v>
-      </c>
-      <c r="M130" s="18">
+      <c r="J130">
+        <v>5.1999999999999997E-5</v>
+      </c>
+      <c r="K130">
+        <v>7.2122999999999996E-3</v>
+      </c>
+      <c r="L130">
+        <v>0</v>
+      </c>
+      <c r="M130">
         <v>1</v>
       </c>
     </row>
@@ -39110,16 +39232,16 @@
       <c r="I131" s="31">
         <v>1</v>
       </c>
-      <c r="J131" s="12">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="K131" s="12">
-        <v>0.30299999999999999</v>
-      </c>
-      <c r="L131" s="12">
-        <v>0</v>
-      </c>
-      <c r="M131" s="18">
+      <c r="J131">
+        <v>0.1024519</v>
+      </c>
+      <c r="K131">
+        <v>0.3032416</v>
+      </c>
+      <c r="L131">
+        <v>0</v>
+      </c>
+      <c r="M131">
         <v>1</v>
       </c>
     </row>
@@ -39151,16 +39273,16 @@
       <c r="I132" s="31">
         <v>1</v>
       </c>
-      <c r="J132" s="12">
-        <v>2E-3</v>
-      </c>
-      <c r="K132" s="12">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="L132" s="12">
-        <v>0</v>
-      </c>
-      <c r="M132" s="18">
+      <c r="J132">
+        <v>2.2859E-3</v>
+      </c>
+      <c r="K132">
+        <v>4.77565E-2</v>
+      </c>
+      <c r="L132">
+        <v>0</v>
+      </c>
+      <c r="M132">
         <v>1</v>
       </c>
     </row>
@@ -39192,16 +39314,16 @@
       <c r="I133" s="31">
         <v>1</v>
       </c>
-      <c r="J133" s="12">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="K133" s="12">
-        <v>0.156</v>
-      </c>
-      <c r="L133" s="12">
-        <v>0</v>
-      </c>
-      <c r="M133" s="18">
+      <c r="J133">
+        <v>2.4917600000000002E-2</v>
+      </c>
+      <c r="K133">
+        <v>0.15587409999999999</v>
+      </c>
+      <c r="L133">
+        <v>0</v>
+      </c>
+      <c r="M133">
         <v>1</v>
       </c>
     </row>
@@ -39233,24 +39355,25 @@
       <c r="I134" s="33">
         <v>1</v>
       </c>
-      <c r="J134" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="K134" s="16">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="L134" s="16">
-        <v>0</v>
-      </c>
-      <c r="M134" s="19">
+      <c r="J134">
+        <v>9.6577E-3</v>
+      </c>
+      <c r="K134">
+        <v>9.7798099999999999E-2</v>
+      </c>
+      <c r="L134">
+        <v>0</v>
+      </c>
+      <c r="M134">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="K105:P123">
-    <sortCondition descending="1" ref="K105"/>
+  <sortState ref="O2:S20">
+    <sortCondition ref="O2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>